<commit_message>
Add accuracy reporting for KNN and SVM in Excel output
- Updated `hasil_klasifikasi.m` to save accuracy metrics for KNN and SVM to the third sheet of the Excel file.
- Created a new table to store method names and their corresponding accuracies, enhancing the output for better analysis.
</commit_message>
<xml_diff>
--- a/hasil_klasifikasi.xlsx
+++ b/hasil_klasifikasi.xlsx
@@ -8,13 +8,14 @@
   <sheets>
     <sheet name="KNN" sheetId="1" r:id="rId2"/>
     <sheet name="SVM" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="142" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="146" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -29,6 +30,18 @@
   </si>
   <si>
     <t>Prediksi</t>
+  </si>
+  <si>
+    <t>Metode</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Akurasi</t>
   </si>
 </sst>
 </file>
@@ -874,4 +887,44 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.453125" customWidth="true"/>
+    <col min="2" max="2" width="11.453125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>79.411764705882348</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>88.235294117647058</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>